<commit_message>
Bulk import user from excel
</commit_message>
<xml_diff>
--- a/invoice-frontend/src/assets/files/user.xlsx
+++ b/invoice-frontend/src/assets/files/user.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>userfirstname</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>Site Supervisor</t>
+  </si>
+  <si>
+    <t>Supervisor</t>
   </si>
 </sst>
 </file>
@@ -435,7 +438,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,7 +528,7 @@
         <v>123</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>

</xml_diff>